<commit_message>
fixed bugs after package update
</commit_message>
<xml_diff>
--- a/Latent Gold/final_analyses.xlsx
+++ b/Latent Gold/final_analyses.xlsx
@@ -15,10 +15,7 @@
     <sheet name="1 class" sheetId="3" r:id="rId1"/>
     <sheet name="2 class" sheetId="1" r:id="rId2"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId3"/>
-  </externalReferences>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -28,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="67">
   <si>
     <t>Model for Choices</t>
   </si>
@@ -234,7 +231,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -271,35 +268,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="12">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="8">
     <dxf>
       <fill>
         <patternFill>
@@ -370,7 +339,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -384,7 +353,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -516,6 +484,11 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-B27E-497B-8D40-1DA06FA84A25}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -647,7 +620,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -715,7 +687,7 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -861,6 +833,11 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-48EB-453B-9D58-8BBE64258A42}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -957,6 +934,11 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-48EB-453B-9D58-8BBE64258A42}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -1155,6 +1137,1367 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="105"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="5"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="2160" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Province</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="2160" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'2 class'!$A$33:$A$37</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>BC</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>MR</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>ON</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>PR</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>QC</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'2 class'!$B$33:$B$37</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>-0.16569999999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.191</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.5400000000000003E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-6.8699999999999997E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-1.9E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-274A-4846-8062-587D13ACDA60}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="26"/>
+        <c:overlap val="-27"/>
+        <c:axId val="69745008"/>
+        <c:axId val="69747920"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="69745008"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="low"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="69747920"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="69747920"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Class Loading</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="low"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="69745008"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr sz="1800"/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+  <c:userShapes r:id="rId3"/>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="105"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="5"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="2160" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Environmental</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Organization</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="2160" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'2 class'!$A$41:$A$43</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>dontknow</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>no</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>yes</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'2 class'!$B$41:$B$43</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.12</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.20349999999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-0.32350000000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-0964-4EB7-916F-8493723A0C92}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="26"/>
+        <c:overlap val="-27"/>
+        <c:axId val="69745008"/>
+        <c:axId val="69747920"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="69745008"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="low"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="69747920"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="69747920"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Class Loading</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="low"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="69745008"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr sz="1800"/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+  <c:userShapes r:id="rId3"/>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="105"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="5"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="2160" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Political Affiliation</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="2160" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'2 class'!$A$47:$A$50</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>CPC</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Liberal</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>NDP/Green</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Other</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'2 class'!$B$47:$B$50</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0.3039</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7.7499999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-0.32800000000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-5.3400000000000003E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-E4EE-4DB5-82F1-DA6726D014A1}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="26"/>
+        <c:overlap val="-27"/>
+        <c:axId val="69745008"/>
+        <c:axId val="69747920"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="69745008"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="low"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="69747920"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="69747920"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Class Loading</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="low"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="69745008"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr sz="1800"/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+  <c:userShapes r:id="rId3"/>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="105"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="5"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="2160" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Age***</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="2160" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>'2 class'!$A$45:$A$45</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'2 class'!$B$45:$B$45</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1.0699999999999999E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-F575-47E3-A998-B5979C10EC3F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="26"/>
+        <c:overlap val="-27"/>
+        <c:axId val="69745008"/>
+        <c:axId val="69747920"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="69745008"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="low"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="69747920"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="69747920"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Class Loading</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="low"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="69745008"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr sz="1800"/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+  <c:userShapes r:id="rId3"/>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -1235,6 +2578,30 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="withinLinearReversed" id="23">
+  <a:schemeClr val="accent3"/>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="withinLinearReversed" id="23">
+  <a:schemeClr val="accent3"/>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="withinLinearReversed" id="23">
+  <a:schemeClr val="accent3"/>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="withinLinearReversed" id="23">
+  <a:schemeClr val="accent3"/>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
@@ -1739,6 +3106,2018 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -2312,138 +5691,590 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>213360</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>110490</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>556260</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>110490</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>69</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Chart 5"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>71</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>91</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="7" name="Chart 6"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>72</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="8" name="Chart 7"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="covariates"/>
-      <sheetName val="2 class"/>
-      <sheetName val="3 class"/>
-      <sheetName val="4 class"/>
-      <sheetName val="5 class"/>
-      <sheetName val="6 class"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1">
-        <row r="7">
-          <cell r="AC7" t="str">
-            <v>Class 1</v>
-          </cell>
-          <cell r="AD7" t="str">
-            <v>Class 2</v>
-          </cell>
-        </row>
-        <row r="8">
-          <cell r="AB8" t="str">
-            <v>Foodprovision</v>
-          </cell>
-          <cell r="AC8">
-            <v>3.8245</v>
-          </cell>
-          <cell r="AD8">
-            <v>2.4173</v>
-          </cell>
-        </row>
-        <row r="9">
-          <cell r="AB9" t="str">
-            <v>NonFoodProducts</v>
-          </cell>
-          <cell r="AC9">
-            <v>0.83140000000000003</v>
-          </cell>
-          <cell r="AD9">
-            <v>6.1100000000000002E-2</v>
-          </cell>
-        </row>
-        <row r="10">
-          <cell r="AB10" t="str">
-            <v>CarbonStorage</v>
-          </cell>
-          <cell r="AC10">
-            <v>1.2885</v>
-          </cell>
-          <cell r="AD10">
-            <v>3.3008000000000002</v>
-          </cell>
-        </row>
-        <row r="11">
-          <cell r="AB11" t="str">
-            <v>CoastalProtection</v>
-          </cell>
-          <cell r="AC11">
-            <v>2.5619000000000001</v>
-          </cell>
-          <cell r="AD11">
-            <v>3.5522999999999998</v>
-          </cell>
-        </row>
-        <row r="12">
-          <cell r="AB12" t="str">
-            <v>CoastalLivelihoods</v>
-          </cell>
-          <cell r="AC12">
-            <v>3.1836000000000002</v>
-          </cell>
-          <cell r="AD12">
-            <v>1.9988999999999999</v>
-          </cell>
-        </row>
-        <row r="13">
-          <cell r="AB13" t="str">
-            <v>TourismandRecreation</v>
-          </cell>
-          <cell r="AC13">
-            <v>1.4201999999999999</v>
-          </cell>
-          <cell r="AD13">
-            <v>0.26179999999999998</v>
-          </cell>
-        </row>
-        <row r="14">
-          <cell r="AB14" t="str">
-            <v>IconicPlacesandSpecies</v>
-          </cell>
-          <cell r="AC14">
-            <v>1.8964000000000001</v>
-          </cell>
-          <cell r="AD14">
-            <v>2.8090000000000002</v>
-          </cell>
-        </row>
-        <row r="15">
-          <cell r="AB15" t="str">
-            <v>CleanWaters</v>
-          </cell>
-          <cell r="AC15">
-            <v>4.3414000000000001</v>
-          </cell>
-          <cell r="AD15">
-            <v>5.3311999999999999</v>
-          </cell>
-        </row>
-        <row r="16">
-          <cell r="AB16" t="str">
-            <v>Biodiversity</v>
-          </cell>
-          <cell r="AC16">
-            <v>1.9572000000000001</v>
-          </cell>
-          <cell r="AD16">
-            <v>3.7126999999999999</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
-      <sheetData sheetId="5"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.76111</cdr:x>
+      <cdr:y>0.21354</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.90694</cdr:x>
+      <cdr:y>0.30104</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="2" name="TextBox 1"/>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="4175760" y="781050"/>
+          <a:ext cx="800100" cy="320040"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip" wrap="square" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="en-US" sz="1600"/>
+            <a:t>Class 1</a:t>
+          </a:r>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.76481</cdr:x>
+      <cdr:y>0.73264</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.91065</cdr:x>
+      <cdr:y>0.82014</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="3" name="TextBox 1"/>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="4196080" y="2679700"/>
+          <a:ext cx="800100" cy="320040"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" wrap="square" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:lvl1pPr marL="0" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="en-US" sz="1600"/>
+            <a:t>Class 2</a:t>
+          </a:r>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+</c:userShapes>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.21389</cdr:x>
+      <cdr:y>0.19062</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.35972</cdr:x>
+      <cdr:y>0.27812</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="2" name="TextBox 1"/>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="1173474" y="697224"/>
+          <a:ext cx="800082" cy="320040"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip" wrap="square" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="en-US" sz="1600"/>
+            <a:t>Class 1</a:t>
+          </a:r>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.21203</cdr:x>
+      <cdr:y>0.75139</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.35787</cdr:x>
+      <cdr:y>0.83889</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="3" name="TextBox 1"/>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="1163294" y="2748284"/>
+          <a:ext cx="800136" cy="320040"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" wrap="square" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:lvl1pPr marL="0" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="en-US" sz="1600"/>
+            <a:t>Class 2</a:t>
+          </a:r>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+</c:userShapes>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.76111</cdr:x>
+      <cdr:y>0.21354</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.90694</cdr:x>
+      <cdr:y>0.30104</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="2" name="TextBox 1"/>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="4175760" y="781050"/>
+          <a:ext cx="800100" cy="320040"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip" wrap="square" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="en-US" sz="1600"/>
+            <a:t>Class 1</a:t>
+          </a:r>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.76481</cdr:x>
+      <cdr:y>0.73264</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.91065</cdr:x>
+      <cdr:y>0.82014</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="3" name="TextBox 1"/>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="4196080" y="2679700"/>
+          <a:ext cx="800100" cy="320040"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" wrap="square" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:lvl1pPr marL="0" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="en-US" sz="1600"/>
+            <a:t>Class 2</a:t>
+          </a:r>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+</c:userShapes>
+</file>
+
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.2125</cdr:x>
+      <cdr:y>0.18437</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.35833</cdr:x>
+      <cdr:y>0.27187</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="2" name="TextBox 1"/>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="1165866" y="674352"/>
+          <a:ext cx="800082" cy="320040"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip" wrap="square" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="en-US" sz="1600"/>
+            <a:t>Class 1</a:t>
+          </a:r>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+</c:userShapes>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3182,8 +7013,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="F56" sqref="F56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>